<commit_message>
update 10 year country info. and keyword freq
</commit_message>
<xml_diff>
--- a/node-with-country-small.xlsx
+++ b/node-with-country-small.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sudos\Dropbox\wos-ss-affiliations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2AFB4D-5198-437E-9DB2-5F77FDA7D351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB555F4-DB69-4731-82F5-F1A7B2F6F5A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1575" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1510" uniqueCount="554">
   <si>
     <t>Id</t>
   </si>
@@ -1678,212 +1678,26 @@
     <t>Tanzania</t>
   </si>
   <si>
+    <t>Tashkent University of Information Technologies</t>
+  </si>
+  <si>
+    <t>Bedford Institute of Oceanography</t>
+  </si>
+  <si>
+    <t>Yellow River Engineering Consulting Co. Ltd.</t>
+  </si>
+  <si>
+    <t>Institute of Mathematics of the Czech Academy of Sciences</t>
+  </si>
+  <si>
+    <t>Escuela Politecnica Superior del Ejercito</t>
+  </si>
+  <si>
+    <t>KDDI Corporation</t>
+  </si>
+  <si>
     <t>Please tell me the nation of the following university or institutes.
-The output the tsv format</t>
-  </si>
-  <si>
-    <t>y_coor</t>
-  </si>
-  <si>
-    <t>University of Peshawar</t>
-  </si>
-  <si>
-    <t>Singapore Management University</t>
-  </si>
-  <si>
-    <t>Inner Mongolia University of Technology</t>
-  </si>
-  <si>
-    <t>Ministry of Agriculture &amp; Rural Affairs</t>
-  </si>
-  <si>
-    <t>Thapar Institute of Engineering &amp; Technology</t>
-  </si>
-  <si>
-    <t>University of Rhode Island</t>
-  </si>
-  <si>
-    <t>Tianjin Medical University</t>
-  </si>
-  <si>
-    <t>University of Tabuk</t>
-  </si>
-  <si>
-    <t>Shimane University</t>
-  </si>
-  <si>
-    <t>University of Melbourne</t>
-  </si>
-  <si>
-    <t>General Research Institute for Nonferrous Metals</t>
-  </si>
-  <si>
-    <t>Henan University of Urban Construction</t>
-  </si>
-  <si>
-    <t>Loughborough University</t>
-  </si>
-  <si>
-    <t>GGS Indraprastha University</t>
-  </si>
-  <si>
-    <t>Zhengzhou University of Technology</t>
-  </si>
-  <si>
-    <t>Henan University of Engineering</t>
-  </si>
-  <si>
-    <t>West Virginia University</t>
-  </si>
-  <si>
-    <t>Iqra University</t>
-  </si>
-  <si>
-    <t>Wuhan Naval University of Engineering</t>
-  </si>
-  <si>
-    <t>Tohoku University</t>
-  </si>
-  <si>
-    <t>University of New Mexico</t>
-  </si>
-  <si>
-    <t>Shenzhen Institute for Advanced Study UESTC</t>
-  </si>
-  <si>
-    <t>University of London</t>
-  </si>
-  <si>
-    <t>University College London</t>
-  </si>
-  <si>
-    <t>National Astronomical Observatory CAS</t>
-  </si>
-  <si>
-    <t>University of California System</t>
-  </si>
-  <si>
-    <t>University of California San Diego</t>
-  </si>
-  <si>
-    <t>University College Cork</t>
-  </si>
-  <si>
-    <t>University of Chinese Academy of Sciences CAS</t>
-  </si>
-  <si>
-    <t>Southwest Forestry University - China</t>
-  </si>
-  <si>
-    <t>University of Texas System</t>
-  </si>
-  <si>
-    <t>University of Texas Rio Grande Valley</t>
-  </si>
-  <si>
-    <t>University System of Georgia</t>
-  </si>
-  <si>
-    <t>Georgia Institute of Technology</t>
-  </si>
-  <si>
-    <t>Institute of Process Engineering CAS</t>
-  </si>
-  <si>
-    <t>N8 Research Partnership</t>
-  </si>
-  <si>
-    <t>Durham University</t>
-  </si>
-  <si>
-    <t>Academy of Mathematics &amp; System Sciences CAS</t>
-  </si>
-  <si>
-    <t>Nanyang Technological University</t>
-  </si>
-  <si>
-    <t>Nanyang Technological University &amp; National Institute of Education (NIE) Singapore</t>
-  </si>
-  <si>
-    <t>University of California Riverside</t>
-  </si>
-  <si>
-    <t>Institute of Chinese Materia Medica CACMS</t>
-  </si>
-  <si>
-    <t>State University System of Florida</t>
-  </si>
-  <si>
-    <t>University of Florida</t>
-  </si>
-  <si>
-    <t>University of North Carolina</t>
-  </si>
-  <si>
-    <t>University of North Carolina Charlotte</t>
-  </si>
-  <si>
-    <t>Changzhi Medical College</t>
-  </si>
-  <si>
-    <t>Touro University California</t>
-  </si>
-  <si>
-    <t>University of Texas Austin</t>
-  </si>
-  <si>
-    <t>University of Quebec</t>
-  </si>
-  <si>
-    <t>UDICE-French Research Universities</t>
-  </si>
-  <si>
-    <t>American University of Middle East</t>
-  </si>
-  <si>
-    <t>Aramco Services Company (ASC)</t>
-  </si>
-  <si>
-    <t>National Institute of Technology Puducherry</t>
-  </si>
-  <si>
-    <t>National University of the Littoral</t>
-  </si>
-  <si>
-    <t>Xishuangbanna Tropical Botanical Garden CAS</t>
-  </si>
-  <si>
-    <t>VA Pittsburgh Healthcare System</t>
-  </si>
-  <si>
-    <t>Pontificia Universidade Catolica de Goias</t>
-  </si>
-  <si>
-    <t>Agilent Technologies</t>
-  </si>
-  <si>
-    <t>Agriculture &amp; Agri Food Canada</t>
-  </si>
-  <si>
-    <t>Asian Institute of Technology</t>
-  </si>
-  <si>
-    <t>Ansteel Group</t>
-  </si>
-  <si>
-    <t>Institute of High Temperature Electrochemistry</t>
-  </si>
-  <si>
-    <t>H Lee Moffitt Cancer Center &amp; Research Institute</t>
-  </si>
-  <si>
-    <t>Institute of Semiconductors Guangdong Academy of Sciences</t>
-  </si>
-  <si>
-    <t>The Northcap University</t>
-  </si>
-  <si>
-    <t>Russian State University of Tourism &amp; Service</t>
+The output the tsv format. The separater is \t</t>
   </si>
 </sst>
 </file>
@@ -2789,15 +2603,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB911729-7732-4CFA-80BF-84AF1A130704}">
-  <dimension ref="A1:C71"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B71"/>
+      <selection activeCell="A2" sqref="A2:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2805,567 +2619,52 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>149</v>
+        <v>3504</v>
       </c>
       <c r="B2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>318</v>
+        <v>3640</v>
       </c>
       <c r="B3" t="s">
-        <v>319</v>
-      </c>
-      <c r="C3" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>423</v>
+        <v>3700</v>
       </c>
       <c r="B4" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>802</v>
+        <v>3920</v>
       </c>
       <c r="B5" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>803</v>
+        <v>4048</v>
       </c>
       <c r="B6" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>804</v>
+        <v>4126</v>
       </c>
       <c r="B7" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>805</v>
-      </c>
-      <c r="B8" t="s">
         <v>552</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>806</v>
-      </c>
-      <c r="B9" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>807</v>
-      </c>
-      <c r="B10" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>808</v>
-      </c>
-      <c r="B11" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>809</v>
-      </c>
-      <c r="B12" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>810</v>
-      </c>
-      <c r="B13" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>811</v>
-      </c>
-      <c r="B14" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>812</v>
-      </c>
-      <c r="B15" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>813</v>
-      </c>
-      <c r="B16" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>814</v>
-      </c>
-      <c r="B17" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>815</v>
-      </c>
-      <c r="B18" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>816</v>
-      </c>
-      <c r="B19" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>817</v>
-      </c>
-      <c r="B20" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>818</v>
-      </c>
-      <c r="B21" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>819</v>
-      </c>
-      <c r="B22" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>820</v>
-      </c>
-      <c r="B23" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>821</v>
-      </c>
-      <c r="B24" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>822</v>
-      </c>
-      <c r="B25" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>823</v>
-      </c>
-      <c r="B26" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>824</v>
-      </c>
-      <c r="B27" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>825</v>
-      </c>
-      <c r="B28" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>826</v>
-      </c>
-      <c r="B29" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>827</v>
-      </c>
-      <c r="B30" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>828</v>
-      </c>
-      <c r="B31" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>829</v>
-      </c>
-      <c r="B32" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>830</v>
-      </c>
-      <c r="B33" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>831</v>
-      </c>
-      <c r="B34" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>832</v>
-      </c>
-      <c r="B35" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>833</v>
-      </c>
-      <c r="B36" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>834</v>
-      </c>
-      <c r="B37" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>835</v>
-      </c>
-      <c r="B38" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>836</v>
-      </c>
-      <c r="B39" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>837</v>
-      </c>
-      <c r="B40" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>838</v>
-      </c>
-      <c r="B41" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>839</v>
-      </c>
-      <c r="B42" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>840</v>
-      </c>
-      <c r="B43" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>841</v>
-      </c>
-      <c r="B44" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>842</v>
-      </c>
-      <c r="B45" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>843</v>
-      </c>
-      <c r="B46" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>844</v>
-      </c>
-      <c r="B47" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>845</v>
-      </c>
-      <c r="B48" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>846</v>
-      </c>
-      <c r="B49" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>847</v>
-      </c>
-      <c r="B50" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>848</v>
-      </c>
-      <c r="B51" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>849</v>
-      </c>
-      <c r="B52" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>850</v>
-      </c>
-      <c r="B53" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>851</v>
-      </c>
-      <c r="B54" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>1415</v>
-      </c>
-      <c r="B55" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>1763</v>
-      </c>
-      <c r="B56" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>2035</v>
-      </c>
-      <c r="B57" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>2051</v>
-      </c>
-      <c r="B58" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>2054</v>
-      </c>
-      <c r="B59" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>2403</v>
-      </c>
-      <c r="B60" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>2827</v>
-      </c>
-      <c r="B61" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>2841</v>
-      </c>
-      <c r="B62" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>2846</v>
-      </c>
-      <c r="B63" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>2848</v>
-      </c>
-      <c r="B64" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>3072</v>
-      </c>
-      <c r="B65" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>3082</v>
-      </c>
-      <c r="B66" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>3085</v>
-      </c>
-      <c r="B67" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>3418</v>
-      </c>
-      <c r="B68" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>3794</v>
-      </c>
-      <c r="B69" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>4835</v>
-      </c>
-      <c r="B70" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>5045</v>
-      </c>
-      <c r="B71" t="s">
-        <v>615</v>
       </c>
     </row>
   </sheetData>
@@ -10401,7 +9700,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>547</v>
+        <v>553</v>
       </c>
     </row>
   </sheetData>

</xml_diff>